<commit_message>
Update Fig 3 data
</commit_message>
<xml_diff>
--- a/data/LanguageFamily.xlsx
+++ b/data/LanguageFamily.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pesavage/Documents/GitHub/sync-coop-song-speech/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/psav050/Documents/GitHub/sync-coop-song-speech/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF92C5A3-BB71-3C40-83E1-EB803CC29402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A269FD-0D90-DC4F-BA25-03D393536907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2320" yWindow="3040" windowWidth="25740" windowHeight="16220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6720" yWindow="2280" windowWidth="18460" windowHeight="16040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SubFamily-level_Final" sheetId="8" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="206">
   <si>
     <t>Afro-Asiatic</t>
   </si>
@@ -663,9 +663,6 @@
     <t>Te Reo Māori (Māori)</t>
   </si>
   <si>
-    <t>Euskara (Basque)</t>
-  </si>
-  <si>
     <t>English [people who stutter]</t>
   </si>
   <si>
@@ -678,9 +675,6 @@
     <t>English [London]</t>
   </si>
   <si>
-    <t>English [NZ]</t>
-  </si>
-  <si>
     <t>Western Farsi</t>
   </si>
   <si>
@@ -693,9 +687,6 @@
     <t>Maasai</t>
   </si>
   <si>
-    <t>Nyunga</t>
-  </si>
-  <si>
     <t>Shipibo-Konibo</t>
   </si>
   <si>
@@ -705,16 +696,52 @@
     <t>(Koreanic?)</t>
   </si>
   <si>
-    <t>(Korean?)</t>
-  </si>
-  <si>
-    <t>(?)</t>
-  </si>
-  <si>
     <t>Finnish</t>
   </si>
   <si>
     <t>Hungarian</t>
+  </si>
+  <si>
+    <t>Mapudungun</t>
+  </si>
+  <si>
+    <t>Dutch</t>
+  </si>
+  <si>
+    <t>English [Hamilton]</t>
+  </si>
+  <si>
+    <t>German [Leipzig]</t>
+  </si>
+  <si>
+    <t>German [Frankfurt]</t>
+  </si>
+  <si>
+    <t>Mosetén-Chimané</t>
+  </si>
+  <si>
+    <t>Mandarin Chinese [Michigan]</t>
+  </si>
+  <si>
+    <t>Tsimane' (Mosetén-Chimané)</t>
+  </si>
+  <si>
+    <t>English [Auckland]</t>
+  </si>
+  <si>
+    <t>Mandarin Chinese [Auckland]</t>
+  </si>
+  <si>
+    <t>Mandarin Chinese [London]</t>
+  </si>
+  <si>
+    <t>Mandarin Chinese [Reading]</t>
+  </si>
+  <si>
+    <t>Newari (Kathmandu Valley Newari)</t>
+  </si>
+  <si>
+    <t>English [Boston]</t>
   </si>
 </sst>
 </file>
@@ -977,7 +1004,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1162,7 +1189,6 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1170,14 +1196,19 @@
     <xf numFmtId="0" fontId="5" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2274,6 +2305,11 @@
     <row r="47" spans="14:14" ht="13" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="G17:I17"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="J3:M3"/>
@@ -2290,11 +2326,6 @@
     <mergeCell ref="J18:M18"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="J20:M20"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="G17:I17"/>
   </mergeCells>
   <phoneticPr fontId="6"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2310,7 +2341,7 @@
   <dimension ref="A1:AR47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2386,266 +2417,261 @@
       <c r="D4" s="24">
         <v>19</v>
       </c>
-      <c r="E4" s="25" t="s">
-        <v>26</v>
+      <c r="E4" s="79" t="s">
+        <v>180</v>
       </c>
       <c r="F4" s="25"/>
       <c r="G4" s="38">
         <v>38</v>
       </c>
-      <c r="H4" s="39" t="s">
-        <v>60</v>
+      <c r="H4" s="85" t="s">
+        <v>186</v>
       </c>
       <c r="I4" s="39"/>
       <c r="J4" s="74"/>
     </row>
-    <row r="5" spans="1:44" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="88" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="88"/>
       <c r="C5" s="88"/>
-      <c r="D5" s="21">
+      <c r="D5" s="24">
         <v>20</v>
       </c>
-      <c r="E5" s="83" t="s">
-        <v>137</v>
-      </c>
-      <c r="F5" s="22"/>
-      <c r="G5" s="38">
-        <v>39</v>
-      </c>
-      <c r="H5" s="86" t="s">
-        <v>188</v>
-      </c>
-      <c r="I5" s="39"/>
-      <c r="J5" s="74"/>
-    </row>
-    <row r="6" spans="1:44" ht="12.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="79" t="s">
+        <v>195</v>
+      </c>
+      <c r="F5" s="25"/>
+      <c r="G5" s="88" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" s="88"/>
+      <c r="I5" s="88"/>
+      <c r="J5" s="88"/>
+    </row>
+    <row r="6" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9">
         <v>2</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>99</v>
+      <c r="B6" s="89" t="s">
+        <v>192</v>
       </c>
       <c r="C6" s="10"/>
-      <c r="D6" s="27">
+      <c r="D6" s="24">
         <v>21</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="79" t="s">
+        <v>196</v>
+      </c>
+      <c r="F6" s="25"/>
+      <c r="G6" s="40">
+        <v>39</v>
+      </c>
+      <c r="H6" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+    </row>
+    <row r="7" spans="1:44" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>3</v>
+      </c>
+      <c r="B7" s="89" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="21">
+        <v>22</v>
+      </c>
+      <c r="E7" s="82" t="s">
+        <v>137</v>
+      </c>
+      <c r="F7" s="22"/>
+      <c r="G7" s="88" t="s">
+        <v>197</v>
+      </c>
+      <c r="H7" s="88"/>
+      <c r="I7" s="88"/>
+      <c r="J7" s="88"/>
+    </row>
+    <row r="8" spans="1:44" ht="12.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="88" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="88"/>
+      <c r="C8" s="88"/>
+      <c r="D8" s="27">
+        <v>23</v>
+      </c>
+      <c r="E8" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="F6" s="29" t="s">
+      <c r="F8" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="G6" s="88" t="s">
-        <v>80</v>
-      </c>
-      <c r="H6" s="88"/>
-      <c r="I6" s="88"/>
-      <c r="J6" s="88"/>
-    </row>
-    <row r="7" spans="1:44" ht="12.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="88" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="88"/>
-      <c r="C7" s="88"/>
-      <c r="D7" s="27">
-        <v>22</v>
-      </c>
-      <c r="E7" s="84" t="s">
-        <v>185</v>
-      </c>
-      <c r="F7" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="G7" s="40">
-        <f>G5+1</f>
+      <c r="G8" s="42">
+        <f>G6+1</f>
         <v>40</v>
       </c>
-      <c r="H7" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-    </row>
-    <row r="8" spans="1:44" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="11">
-        <v>3</v>
-      </c>
-      <c r="B8" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="C8" s="64"/>
-      <c r="D8" s="24">
-        <v>23</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="G8" s="88" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="88"/>
-      <c r="I8" s="88"/>
-      <c r="J8" s="88"/>
+      <c r="H8" s="77" t="s">
+        <v>199</v>
+      </c>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
       <c r="AB8" s="3"/>
       <c r="AC8" s="3"/>
     </row>
-    <row r="9" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:44" ht="12.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>4</v>
       </c>
       <c r="B9" s="75" t="s">
-        <v>114</v>
+        <v>176</v>
       </c>
       <c r="C9" s="64"/>
-      <c r="D9" s="24">
-        <f>D8+1</f>
+      <c r="D9" s="27">
         <v>24</v>
       </c>
-      <c r="E9" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="25"/>
-      <c r="G9" s="42">
-        <f>G7+1</f>
-        <v>41</v>
-      </c>
-      <c r="H9" s="77" t="s">
-        <v>189</v>
-      </c>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
+      <c r="E9" s="83" t="s">
+        <v>183</v>
+      </c>
+      <c r="F9" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" s="88" t="s">
+        <v>72</v>
+      </c>
+      <c r="H9" s="88"/>
+      <c r="I9" s="88"/>
+      <c r="J9" s="88"/>
       <c r="AB9" s="3"/>
       <c r="AC9" s="3"/>
     </row>
-    <row r="10" spans="1:44" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="60">
+    <row r="10" spans="1:44" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="11">
         <v>5</v>
       </c>
-      <c r="B10" s="81" t="s">
-        <v>115</v>
-      </c>
-      <c r="C10" s="65"/>
+      <c r="B10" s="75" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" s="64"/>
       <c r="D10" s="24">
-        <f>D9+1</f>
         <v>25</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10" s="25"/>
-      <c r="G10" s="88" t="s">
-        <v>72</v>
-      </c>
-      <c r="H10" s="88"/>
-      <c r="I10" s="88"/>
-      <c r="J10" s="88"/>
+        <v>17</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="G10" s="44">
+        <f>G8+1</f>
+        <v>41</v>
+      </c>
+      <c r="H10" s="86" t="s">
+        <v>187</v>
+      </c>
+      <c r="I10" s="45"/>
+      <c r="J10" s="45"/>
       <c r="AB10" s="3"/>
       <c r="AC10" s="3"/>
     </row>
-    <row r="11" spans="1:44" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="88" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="88"/>
-      <c r="C11" s="88"/>
+    <row r="11" spans="1:44" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="60">
+        <v>6</v>
+      </c>
+      <c r="B11" s="81" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" s="65"/>
       <c r="D11" s="24">
-        <f t="shared" ref="D11:D19" si="0">D10+1</f>
         <v>26</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="F11" s="25"/>
-      <c r="G11" s="44">
-        <f>G9+1</f>
-        <v>42</v>
-      </c>
-      <c r="H11" s="87" t="s">
-        <v>190</v>
-      </c>
-      <c r="I11" s="45"/>
-      <c r="J11" s="45"/>
+      <c r="G11" s="88" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="88"/>
+      <c r="I11" s="88"/>
+      <c r="J11" s="88"/>
       <c r="AB11" s="3"/>
       <c r="AC11" s="3"/>
     </row>
-    <row r="12" spans="1:44" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13">
-        <v>6</v>
-      </c>
-      <c r="B12" s="78" t="s">
-        <v>177</v>
-      </c>
-      <c r="C12" s="14"/>
+    <row r="12" spans="1:44" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="88" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="88"/>
+      <c r="C12" s="88"/>
       <c r="D12" s="24">
-        <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="E12" s="79" t="s">
-        <v>186</v>
+      <c r="E12" s="25" t="s">
+        <v>52</v>
       </c>
       <c r="F12" s="25"/>
-      <c r="G12" s="88" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="88"/>
-      <c r="I12" s="88"/>
-      <c r="J12" s="88"/>
+      <c r="G12" s="50">
+        <v>42</v>
+      </c>
+      <c r="H12" s="91" t="s">
+        <v>198</v>
+      </c>
+      <c r="I12" s="49"/>
+      <c r="J12" s="69"/>
       <c r="AB12" s="3"/>
       <c r="AC12" s="3"/>
     </row>
-    <row r="13" spans="1:44" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="13">
+    <row r="13" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="92">
         <v>7</v>
       </c>
       <c r="B13" s="78" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="24">
-        <f>D12+1</f>
         <v>28</v>
       </c>
-      <c r="E13" s="25" t="s">
-        <v>71</v>
+      <c r="E13" s="79" t="s">
+        <v>184</v>
       </c>
       <c r="F13" s="25"/>
-      <c r="G13" s="71">
+      <c r="G13" s="50">
         <v>43</v>
       </c>
-      <c r="H13" s="72" t="s">
-        <v>63</v>
-      </c>
-      <c r="I13" s="72"/>
-      <c r="J13" s="73"/>
+      <c r="H13" s="91" t="s">
+        <v>201</v>
+      </c>
+      <c r="I13" s="49"/>
+      <c r="J13" s="69"/>
       <c r="AB13" s="3"/>
       <c r="AC13" s="3"/>
     </row>
     <row r="14" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="88" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="88"/>
-      <c r="C14" s="88"/>
+      <c r="A14" s="92">
+        <v>8</v>
+      </c>
+      <c r="B14" s="78" t="s">
+        <v>178</v>
+      </c>
+      <c r="C14" s="14"/>
       <c r="D14" s="24">
-        <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="E14" s="25" t="s">
-        <v>47</v>
+      <c r="E14" s="79" t="s">
+        <v>150</v>
       </c>
       <c r="F14" s="25"/>
       <c r="G14" s="50">
         <v>44</v>
       </c>
-      <c r="H14" s="49" t="s">
-        <v>43</v>
+      <c r="H14" s="91" t="s">
+        <v>202</v>
       </c>
       <c r="I14" s="49"/>
       <c r="J14" s="69"/>
@@ -2653,196 +2679,191 @@
       <c r="AC14" s="3"/>
     </row>
     <row r="15" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="15">
-        <v>8</v>
-      </c>
-      <c r="B15" s="82" t="s">
-        <v>179</v>
-      </c>
-      <c r="C15" s="16"/>
+      <c r="A15" s="88" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="88"/>
+      <c r="C15" s="88"/>
       <c r="D15" s="24">
         <v>30</v>
       </c>
-      <c r="E15" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="26" t="s">
-        <v>87</v>
-      </c>
-      <c r="G15" s="88" t="s">
-        <v>91</v>
-      </c>
-      <c r="H15" s="88"/>
-      <c r="I15" s="88"/>
-      <c r="J15" s="88"/>
+      <c r="E15" s="79" t="s">
+        <v>148</v>
+      </c>
+      <c r="F15" s="25"/>
+      <c r="G15" s="50">
+        <v>45</v>
+      </c>
+      <c r="H15" s="91" t="s">
+        <v>203</v>
+      </c>
+      <c r="I15" s="49"/>
+      <c r="J15" s="69"/>
       <c r="AB15" s="3"/>
       <c r="AC15" s="3"/>
     </row>
     <row r="16" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="88" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="88"/>
-      <c r="C16" s="88"/>
+      <c r="A16" s="17">
+        <v>9</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="18"/>
       <c r="D16" s="24">
-        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="F16" s="25"/>
-      <c r="G16" s="58">
-        <f>G14+1</f>
-        <v>45</v>
-      </c>
-      <c r="H16" s="59" t="s">
-        <v>92</v>
-      </c>
-      <c r="I16" s="59"/>
-      <c r="J16" s="59"/>
+        <v>24</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="G16" s="50">
+        <v>46</v>
+      </c>
+      <c r="H16" s="91" t="s">
+        <v>204</v>
+      </c>
+      <c r="I16" s="49"/>
+      <c r="J16" s="69"/>
       <c r="AB16" s="3"/>
       <c r="AC16" s="3"/>
     </row>
     <row r="17" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="17">
-        <v>9</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="C17" s="18"/>
+      <c r="A17" s="88" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="88"/>
+      <c r="C17" s="88"/>
       <c r="D17" s="24">
-        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="F17" s="25"/>
       <c r="G17" s="88" t="s">
-        <v>14</v>
+        <v>91</v>
       </c>
       <c r="H17" s="88"/>
       <c r="I17" s="88"/>
       <c r="J17" s="88"/>
     </row>
     <row r="18" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="88" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="88"/>
-      <c r="C18" s="88"/>
+      <c r="A18" s="19">
+        <v>10</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="20"/>
       <c r="D18" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D18:D19" si="0">D17+1</f>
         <v>33</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F18" s="25"/>
-      <c r="G18" s="56">
+      <c r="G18" s="58">
         <f>G16+1</f>
-        <v>46</v>
-      </c>
-      <c r="H18" s="57" t="s">
-        <v>36</v>
-      </c>
-      <c r="I18" s="57"/>
-      <c r="J18" s="57"/>
+        <v>47</v>
+      </c>
+      <c r="H18" s="59" t="s">
+        <v>92</v>
+      </c>
+      <c r="I18" s="59"/>
+      <c r="J18" s="59"/>
     </row>
     <row r="19" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="19">
-        <v>10</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="20"/>
+      <c r="A19" s="88" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="88"/>
+      <c r="C19" s="88"/>
       <c r="D19" s="24">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>104</v>
+        <v>32</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="88" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H19" s="88"/>
       <c r="I19" s="88"/>
       <c r="J19" s="88"/>
     </row>
     <row r="20" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="88" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="88"/>
-      <c r="C20" s="88"/>
+      <c r="A20" s="24">
+        <v>11</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>83</v>
+      </c>
       <c r="D20" s="88" t="s">
         <v>5</v>
       </c>
       <c r="E20" s="88"/>
       <c r="F20" s="88"/>
-      <c r="G20" s="53">
-        <v>47</v>
-      </c>
-      <c r="H20" s="55" t="s">
-        <v>16</v>
-      </c>
-      <c r="I20" s="55"/>
-      <c r="J20" s="55"/>
-    </row>
-    <row r="21" spans="1:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="21">
-        <v>11</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="23" t="s">
-        <v>82</v>
-      </c>
+      <c r="G20" s="56">
+        <f>G18+1</f>
+        <v>48</v>
+      </c>
+      <c r="H20" s="57" t="s">
+        <v>36</v>
+      </c>
+      <c r="I20" s="57"/>
+      <c r="J20" s="57"/>
+    </row>
+    <row r="21" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="24">
+        <v>12</v>
+      </c>
+      <c r="B21" s="79" t="s">
+        <v>193</v>
+      </c>
+      <c r="C21" s="25"/>
       <c r="D21" s="32">
         <f>D19+1</f>
         <v>35</v>
       </c>
-      <c r="E21" s="85" t="s">
-        <v>187</v>
+      <c r="E21" s="84" t="s">
+        <v>185</v>
       </c>
       <c r="F21" s="33"/>
       <c r="G21" s="88" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="H21" s="88"/>
       <c r="I21" s="88"/>
       <c r="J21" s="88"/>
     </row>
-    <row r="22" spans="1:16" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="24">
-        <v>12</v>
-      </c>
-      <c r="B22" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="D22" s="32">
-        <f>D21+1</f>
-        <v>36</v>
-      </c>
-      <c r="E22" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="F22" s="33"/>
+        <f t="shared" ref="A22:A27" si="1">A21+1</f>
+        <v>13</v>
+      </c>
+      <c r="B22" s="79" t="s">
+        <v>200</v>
+      </c>
+      <c r="C22" s="25"/>
+      <c r="D22" s="88" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="88"/>
+      <c r="F22" s="88"/>
       <c r="G22" s="51">
-        <f>G20+1</f>
-        <v>48</v>
-      </c>
-      <c r="H22" s="90" t="s">
-        <v>195</v>
+        <v>49</v>
+      </c>
+      <c r="H22" s="87" t="s">
+        <v>190</v>
       </c>
       <c r="I22" s="52"/>
       <c r="J22" s="52"/>
@@ -2854,96 +2875,82 @@
     </row>
     <row r="23" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A23" s="24">
-        <v>13</v>
+        <f t="shared" si="1"/>
+        <v>14</v>
       </c>
       <c r="B23" s="79" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C23" s="25"/>
-      <c r="D23" s="88" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23" s="88"/>
-      <c r="F23" s="88"/>
+      <c r="D23" s="34">
+        <v>36</v>
+      </c>
+      <c r="E23" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="35"/>
       <c r="G23" s="51">
-        <v>49</v>
-      </c>
-      <c r="H23" s="90" t="s">
-        <v>196</v>
+        <v>50</v>
+      </c>
+      <c r="H23" s="87" t="s">
+        <v>191</v>
       </c>
       <c r="I23" s="52"/>
       <c r="J23" s="52"/>
     </row>
     <row r="24" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A24" s="24">
-        <f t="shared" ref="A24:A28" si="1">A23+1</f>
-        <v>14</v>
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
       <c r="B24" s="79" t="s">
-        <v>182</v>
+        <v>205</v>
       </c>
       <c r="C24" s="25"/>
-      <c r="D24" s="34">
-        <f>D22+1</f>
-        <v>37</v>
-      </c>
-      <c r="E24" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="F24" s="35"/>
+      <c r="D24" s="88" t="s">
+        <v>189</v>
+      </c>
+      <c r="E24" s="88"/>
+      <c r="F24" s="88"/>
     </row>
     <row r="25" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A25" s="24">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B25" s="79" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C25" s="25"/>
-      <c r="D25" s="88" t="s">
-        <v>192</v>
-      </c>
-      <c r="E25" s="88"/>
-      <c r="F25" s="88"/>
+      <c r="D25" s="36">
+        <v>37</v>
+      </c>
+      <c r="E25" s="90" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="90"/>
     </row>
     <row r="26" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A26" s="24">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B26" s="79" t="s">
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="C26" s="25"/>
-      <c r="D26" s="36" t="s">
-        <v>194</v>
-      </c>
-      <c r="E26" s="89" t="s">
-        <v>193</v>
-      </c>
-      <c r="F26" s="89"/>
     </row>
     <row r="27" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A27" s="24">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B27" s="79" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C27" s="25"/>
     </row>
-    <row r="28" spans="1:16" ht="14" x14ac:dyDescent="0.2">
-      <c r="A28" s="24">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="B28" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="C28" s="25"/>
-    </row>
+    <row r="28" spans="1:16" ht="13" x14ac:dyDescent="0.15"/>
     <row r="29" spans="1:16" ht="13" x14ac:dyDescent="0.15"/>
     <row r="30" spans="1:16" ht="13" x14ac:dyDescent="0.15"/>
     <row r="31" spans="1:16" ht="13" x14ac:dyDescent="0.15"/>
@@ -2974,28 +2981,26 @@
     <row r="46" spans="11:11" ht="13" x14ac:dyDescent="0.15"/>
     <row r="47" spans="11:11" ht="13" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="19">
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A8:C8"/>
     <mergeCell ref="G21:J21"/>
     <mergeCell ref="G3:J3"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A19:C19"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="D20:F20"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="G11:J11"/>
     <mergeCell ref="G17:J17"/>
     <mergeCell ref="G19:J19"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A7:C7"/>
   </mergeCells>
   <phoneticPr fontId="6"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>